<commit_message>
feat: add more diseases
</commit_message>
<xml_diff>
--- a/data_demo.xlsx
+++ b/data_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\guess-disease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EF44A3-E402-44D6-AA85-6DCB3B2D82FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCD1CA3-9CFB-421D-8D82-F8CAE574A42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EDC1453C-E04D-46A8-B4D3-D1964BBBCD97}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="75">
   <si>
     <t>Demam</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Batuk Kering</t>
   </si>
   <si>
-    <t>Suara Serak</t>
-  </si>
-  <si>
     <t>Penyakit</t>
   </si>
   <si>
@@ -172,6 +169,96 @@
   </si>
   <si>
     <t>Nyeri pada wajah</t>
+  </si>
+  <si>
+    <t>Suara serak</t>
+  </si>
+  <si>
+    <t>Dyspepsia</t>
+  </si>
+  <si>
+    <t>Nyeri ulu hati</t>
+  </si>
+  <si>
+    <t>Nyeri memberat setelah makan</t>
+  </si>
+  <si>
+    <t>Regurgitasi (Rasa pahit/asam di mulut)</t>
+  </si>
+  <si>
+    <t>Perut kembung</t>
+  </si>
+  <si>
+    <t>Mual</t>
+  </si>
+  <si>
+    <t>Anorexia (hilang nafsu makan)</t>
+  </si>
+  <si>
+    <t>GERD</t>
+  </si>
+  <si>
+    <t>Rasa panas di dada</t>
+  </si>
+  <si>
+    <t>Muntah</t>
+  </si>
+  <si>
+    <t>Batuk</t>
+  </si>
+  <si>
+    <t>Appendicitis Akut</t>
+  </si>
+  <si>
+    <t>Nyeri perut kanan bawah</t>
+  </si>
+  <si>
+    <t>Nyeri perut kanan atas</t>
+  </si>
+  <si>
+    <t>Durasi demam</t>
+  </si>
+  <si>
+    <t>Diare (BAB encer ≥3x/hari)</t>
+  </si>
+  <si>
+    <t>Konstipasi</t>
+  </si>
+  <si>
+    <t>Gastroenteritis Akut</t>
+  </si>
+  <si>
+    <t>Nyeri perut (tidak terlokalisir)</t>
+  </si>
+  <si>
+    <t>Demam Tifoid</t>
+  </si>
+  <si>
+    <t>Pankreatitis Akut</t>
+  </si>
+  <si>
+    <t>jarang</t>
+  </si>
+  <si>
+    <t>Cholecystitis</t>
+  </si>
+  <si>
+    <t>Kekuningan pada Tubuh (mata/badan)</t>
+  </si>
+  <si>
+    <t>Hepatitis</t>
+  </si>
+  <si>
+    <t>Perut membuncit</t>
+  </si>
+  <si>
+    <t>Pucat (Anemia)</t>
+  </si>
+  <si>
+    <t>Ascariasis</t>
+  </si>
+  <si>
+    <t>sangat sering</t>
   </si>
 </sst>
 </file>
@@ -532,11 +619,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1104B6-B40D-43C4-83C1-9C88DDF12283}">
-  <dimension ref="A1:D133"/>
+  <dimension ref="A1:D233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C144" sqref="C144"/>
+      <pane ySplit="1" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A233" sqref="A233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,16 +636,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -621,7 +708,7 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -679,7 +766,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -737,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -1122,7 +1209,7 @@
         <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D52" t="s">
         <v>16</v>
@@ -1180,7 +1267,7 @@
         <v>11</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D57" t="s">
         <v>13</v>
@@ -1238,7 +1325,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D62" t="s">
         <v>13</v>
@@ -1428,7 +1515,7 @@
         <v>10</v>
       </c>
       <c r="C79" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D79" t="s">
         <v>16</v>
@@ -1505,7 +1592,7 @@
         <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D86" t="s">
         <v>16</v>
@@ -1563,7 +1650,7 @@
         <v>11</v>
       </c>
       <c r="C91" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D91" t="s">
         <v>13</v>
@@ -1621,7 +1708,7 @@
         <v>10</v>
       </c>
       <c r="C96" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D96" t="s">
         <v>13</v>
@@ -1852,7 +1939,7 @@
         <v>36</v>
       </c>
       <c r="B117" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D117" t="s">
         <v>13</v>
@@ -2032,6 +2119,1106 @@
       </c>
       <c r="D133" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>46</v>
+      </c>
+      <c r="B134" t="s">
+        <v>47</v>
+      </c>
+      <c r="D134" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>46</v>
+      </c>
+      <c r="B135" t="s">
+        <v>48</v>
+      </c>
+      <c r="D135" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>46</v>
+      </c>
+      <c r="B136" t="s">
+        <v>49</v>
+      </c>
+      <c r="D136" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>46</v>
+      </c>
+      <c r="B137" t="s">
+        <v>50</v>
+      </c>
+      <c r="D137" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>46</v>
+      </c>
+      <c r="B138" t="s">
+        <v>51</v>
+      </c>
+      <c r="D138" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>46</v>
+      </c>
+      <c r="B139" t="s">
+        <v>52</v>
+      </c>
+      <c r="D139" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>53</v>
+      </c>
+      <c r="B140" t="s">
+        <v>47</v>
+      </c>
+      <c r="D140" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>53</v>
+      </c>
+      <c r="B141" t="s">
+        <v>48</v>
+      </c>
+      <c r="D141" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>53</v>
+      </c>
+      <c r="B142" t="s">
+        <v>54</v>
+      </c>
+      <c r="D142" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>53</v>
+      </c>
+      <c r="B143" t="s">
+        <v>49</v>
+      </c>
+      <c r="D143" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>53</v>
+      </c>
+      <c r="B144" t="s">
+        <v>50</v>
+      </c>
+      <c r="D144" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>53</v>
+      </c>
+      <c r="B145" t="s">
+        <v>51</v>
+      </c>
+      <c r="D145" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>53</v>
+      </c>
+      <c r="B146" t="s">
+        <v>55</v>
+      </c>
+      <c r="D146" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>53</v>
+      </c>
+      <c r="B147" t="s">
+        <v>56</v>
+      </c>
+      <c r="D147" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>53</v>
+      </c>
+      <c r="B148" t="s">
+        <v>45</v>
+      </c>
+      <c r="D148" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>53</v>
+      </c>
+      <c r="B149" t="s">
+        <v>20</v>
+      </c>
+      <c r="D149" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>53</v>
+      </c>
+      <c r="B150" t="s">
+        <v>52</v>
+      </c>
+      <c r="D150" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>57</v>
+      </c>
+      <c r="B151" t="s">
+        <v>58</v>
+      </c>
+      <c r="D151" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>57</v>
+      </c>
+      <c r="B152" t="s">
+        <v>47</v>
+      </c>
+      <c r="D152" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>57</v>
+      </c>
+      <c r="B153" t="s">
+        <v>59</v>
+      </c>
+      <c r="D153" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>57</v>
+      </c>
+      <c r="B154" t="s">
+        <v>50</v>
+      </c>
+      <c r="D154" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>57</v>
+      </c>
+      <c r="B155" t="s">
+        <v>51</v>
+      </c>
+      <c r="D155" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>57</v>
+      </c>
+      <c r="B156" t="s">
+        <v>55</v>
+      </c>
+      <c r="D156" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>57</v>
+      </c>
+      <c r="B157" t="s">
+        <v>0</v>
+      </c>
+      <c r="D157" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>57</v>
+      </c>
+      <c r="B158" t="s">
+        <v>60</v>
+      </c>
+      <c r="C158" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>57</v>
+      </c>
+      <c r="B159" t="s">
+        <v>52</v>
+      </c>
+      <c r="D159" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>57</v>
+      </c>
+      <c r="B160" t="s">
+        <v>61</v>
+      </c>
+      <c r="D160" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>57</v>
+      </c>
+      <c r="B161" t="s">
+        <v>62</v>
+      </c>
+      <c r="D161" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>63</v>
+      </c>
+      <c r="B162" t="s">
+        <v>64</v>
+      </c>
+      <c r="D162" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>63</v>
+      </c>
+      <c r="B163" t="s">
+        <v>50</v>
+      </c>
+      <c r="D163" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>63</v>
+      </c>
+      <c r="B164" t="s">
+        <v>51</v>
+      </c>
+      <c r="D164" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>63</v>
+      </c>
+      <c r="B165" t="s">
+        <v>55</v>
+      </c>
+      <c r="D165" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>63</v>
+      </c>
+      <c r="B166" t="s">
+        <v>0</v>
+      </c>
+      <c r="D166" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>63</v>
+      </c>
+      <c r="B167" t="s">
+        <v>60</v>
+      </c>
+      <c r="C167" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>63</v>
+      </c>
+      <c r="B168" t="s">
+        <v>52</v>
+      </c>
+      <c r="D168" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>63</v>
+      </c>
+      <c r="B169" t="s">
+        <v>61</v>
+      </c>
+      <c r="D169" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>63</v>
+      </c>
+      <c r="B170" t="s">
+        <v>62</v>
+      </c>
+      <c r="D170" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>63</v>
+      </c>
+      <c r="B171" t="s">
+        <v>11</v>
+      </c>
+      <c r="D171" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>65</v>
+      </c>
+      <c r="B172" t="s">
+        <v>58</v>
+      </c>
+      <c r="D172" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>65</v>
+      </c>
+      <c r="B173" t="s">
+        <v>47</v>
+      </c>
+      <c r="D173" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>65</v>
+      </c>
+      <c r="B174" t="s">
+        <v>64</v>
+      </c>
+      <c r="D174" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>65</v>
+      </c>
+      <c r="B175" t="s">
+        <v>50</v>
+      </c>
+      <c r="D175" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>65</v>
+      </c>
+      <c r="B176" t="s">
+        <v>51</v>
+      </c>
+      <c r="D176" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>65</v>
+      </c>
+      <c r="B177" t="s">
+        <v>55</v>
+      </c>
+      <c r="D177" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>65</v>
+      </c>
+      <c r="B178" t="s">
+        <v>0</v>
+      </c>
+      <c r="D178" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>65</v>
+      </c>
+      <c r="B179" t="s">
+        <v>60</v>
+      </c>
+      <c r="C179" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>65</v>
+      </c>
+      <c r="B180" t="s">
+        <v>52</v>
+      </c>
+      <c r="D180" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>65</v>
+      </c>
+      <c r="B181" t="s">
+        <v>61</v>
+      </c>
+      <c r="D181" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>65</v>
+      </c>
+      <c r="B182" t="s">
+        <v>62</v>
+      </c>
+      <c r="D182" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>65</v>
+      </c>
+      <c r="B183" t="s">
+        <v>10</v>
+      </c>
+      <c r="D183" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>65</v>
+      </c>
+      <c r="B184" t="s">
+        <v>11</v>
+      </c>
+      <c r="D184" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>66</v>
+      </c>
+      <c r="B185" t="s">
+        <v>47</v>
+      </c>
+      <c r="D185" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>66</v>
+      </c>
+      <c r="B186" t="s">
+        <v>64</v>
+      </c>
+      <c r="D186" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>66</v>
+      </c>
+      <c r="B187" t="s">
+        <v>48</v>
+      </c>
+      <c r="D187" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>66</v>
+      </c>
+      <c r="B188" t="s">
+        <v>50</v>
+      </c>
+      <c r="D188" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>66</v>
+      </c>
+      <c r="B189" t="s">
+        <v>51</v>
+      </c>
+      <c r="D189" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>66</v>
+      </c>
+      <c r="B190" t="s">
+        <v>55</v>
+      </c>
+      <c r="D190" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>66</v>
+      </c>
+      <c r="B191" t="s">
+        <v>20</v>
+      </c>
+      <c r="D191" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>66</v>
+      </c>
+      <c r="B192" t="s">
+        <v>0</v>
+      </c>
+      <c r="D192" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>66</v>
+      </c>
+      <c r="B193" t="s">
+        <v>60</v>
+      </c>
+      <c r="C193" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>66</v>
+      </c>
+      <c r="B194" t="s">
+        <v>52</v>
+      </c>
+      <c r="D194" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>66</v>
+      </c>
+      <c r="B195" t="s">
+        <v>61</v>
+      </c>
+      <c r="D195" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>66</v>
+      </c>
+      <c r="B196" t="s">
+        <v>62</v>
+      </c>
+      <c r="D196" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>68</v>
+      </c>
+      <c r="B197" t="s">
+        <v>64</v>
+      </c>
+      <c r="D197" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>68</v>
+      </c>
+      <c r="B198" t="s">
+        <v>59</v>
+      </c>
+      <c r="D198" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>68</v>
+      </c>
+      <c r="B199" t="s">
+        <v>48</v>
+      </c>
+      <c r="D199" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>68</v>
+      </c>
+      <c r="B200" t="s">
+        <v>50</v>
+      </c>
+      <c r="D200" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>68</v>
+      </c>
+      <c r="B201" t="s">
+        <v>51</v>
+      </c>
+      <c r="D201" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>68</v>
+      </c>
+      <c r="B202" t="s">
+        <v>55</v>
+      </c>
+      <c r="D202" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>68</v>
+      </c>
+      <c r="B203" t="s">
+        <v>0</v>
+      </c>
+      <c r="D203" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>68</v>
+      </c>
+      <c r="B204" t="s">
+        <v>60</v>
+      </c>
+      <c r="C204" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>68</v>
+      </c>
+      <c r="B205" t="s">
+        <v>52</v>
+      </c>
+      <c r="D205" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>68</v>
+      </c>
+      <c r="B206" t="s">
+        <v>69</v>
+      </c>
+      <c r="D206" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>70</v>
+      </c>
+      <c r="B207" t="s">
+        <v>59</v>
+      </c>
+      <c r="D207" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>70</v>
+      </c>
+      <c r="B208" t="s">
+        <v>48</v>
+      </c>
+      <c r="D208" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>70</v>
+      </c>
+      <c r="B209" t="s">
+        <v>50</v>
+      </c>
+      <c r="D209" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>70</v>
+      </c>
+      <c r="B210" t="s">
+        <v>71</v>
+      </c>
+      <c r="D210" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>70</v>
+      </c>
+      <c r="B211" t="s">
+        <v>51</v>
+      </c>
+      <c r="D211" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>70</v>
+      </c>
+      <c r="B212" t="s">
+        <v>55</v>
+      </c>
+      <c r="D212" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>70</v>
+      </c>
+      <c r="B213" t="s">
+        <v>20</v>
+      </c>
+      <c r="D213" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
+        <v>70</v>
+      </c>
+      <c r="B214" t="s">
+        <v>0</v>
+      </c>
+      <c r="D214" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>70</v>
+      </c>
+      <c r="B215" t="s">
+        <v>60</v>
+      </c>
+      <c r="C215" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>70</v>
+      </c>
+      <c r="B216" t="s">
+        <v>52</v>
+      </c>
+      <c r="D216" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>70</v>
+      </c>
+      <c r="B217" t="s">
+        <v>32</v>
+      </c>
+      <c r="D217" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>70</v>
+      </c>
+      <c r="B218" t="s">
+        <v>11</v>
+      </c>
+      <c r="D218" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>70</v>
+      </c>
+      <c r="B219" t="s">
+        <v>69</v>
+      </c>
+      <c r="D219" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>70</v>
+      </c>
+      <c r="B220" t="s">
+        <v>72</v>
+      </c>
+      <c r="D220" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>73</v>
+      </c>
+      <c r="B221" t="s">
+        <v>64</v>
+      </c>
+      <c r="D221" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>73</v>
+      </c>
+      <c r="B222" t="s">
+        <v>50</v>
+      </c>
+      <c r="D222" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>73</v>
+      </c>
+      <c r="B223" t="s">
+        <v>71</v>
+      </c>
+      <c r="D223" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>73</v>
+      </c>
+      <c r="B224" t="s">
+        <v>51</v>
+      </c>
+      <c r="D224" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>73</v>
+      </c>
+      <c r="B225" t="s">
+        <v>55</v>
+      </c>
+      <c r="D225" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>73</v>
+      </c>
+      <c r="B226" t="s">
+        <v>56</v>
+      </c>
+      <c r="D226" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>73</v>
+      </c>
+      <c r="B227" t="s">
+        <v>0</v>
+      </c>
+      <c r="D227" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>73</v>
+      </c>
+      <c r="B228" t="s">
+        <v>60</v>
+      </c>
+      <c r="C228" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>73</v>
+      </c>
+      <c r="B229" t="s">
+        <v>52</v>
+      </c>
+      <c r="D229" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>73</v>
+      </c>
+      <c r="B230" t="s">
+        <v>32</v>
+      </c>
+      <c r="D230" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>73</v>
+      </c>
+      <c r="B231" t="s">
+        <v>61</v>
+      </c>
+      <c r="D231" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>73</v>
+      </c>
+      <c r="B232" t="s">
+        <v>62</v>
+      </c>
+      <c r="D232" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>73</v>
+      </c>
+      <c r="B233" t="s">
+        <v>72</v>
+      </c>
+      <c r="D233" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
conf: change sheet name
</commit_message>
<xml_diff>
--- a/data_demo.xlsx
+++ b/data_demo.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\guess-disease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFC708D-BD51-4EED-9913-2012AFFADCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1F690F-5F55-4891-B029-8CF9F5A2F50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{EDC1453C-E04D-46A8-B4D3-D1964BBBCD97}"/>
   </bookViews>
   <sheets>
     <sheet name="SymptomTable" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="SubsymptomTable" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1104B6-B40D-43C4-83C1-9C88DDF12283}">
   <dimension ref="A1:D233"/>
   <sheetViews>
-    <sheetView zoomScale="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A214" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A233" sqref="A233"/>
     </sheetView>
   </sheetViews>
@@ -3238,7 +3238,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>